<commit_message>
Updated some file names and names of Excel output columns
</commit_message>
<xml_diff>
--- a/ISATab2MCDS_DCL/DCLConversionEval.xlsx
+++ b/ISATab2MCDS_DCL/DCLConversionEval.xlsx
@@ -23,10 +23,10 @@
     <t>Passed Validation</t>
   </si>
   <si>
-    <t>Total Entities in New File</t>
-  </si>
-  <si>
-    <t>Num of Issues in New File</t>
+    <t>Total Data Entities in Converted File</t>
+  </si>
+  <si>
+    <t>Num of Issues in Converted File</t>
   </si>
   <si>
     <t>MCDS_L_0000000003</t>

</xml_diff>